<commit_message>
Modified first 10 rows based on recent estimates.
</commit_message>
<xml_diff>
--- a/computing_model_2016-11.xlsx
+++ b/computing_model_2016-11.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="0" windowWidth="29420" windowHeight="19220" tabRatio="991"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="29420" windowHeight="19220" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>CPU-s/event</t>
   </si>
   <si>
-    <t>Time to reconstruct a single event on a 2.8 GHz Nehalem machine, per thread, from Simon's email of 1/31/2011</t>
-  </si>
-  <si>
     <t>single Pass 1 CPU needed</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>bytes</t>
   </si>
   <si>
-    <t>size of a single raw event</t>
-  </si>
-  <si>
     <t>raw instantaneous storage rate</t>
   </si>
   <si>
@@ -491,6 +485,12 @@
   </si>
   <si>
     <t>total data to tape (PB)</t>
+  </si>
+  <si>
+    <t>Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</t>
+  </si>
+  <si>
+    <t>size of a single raw event. Actual Spring 2016 data is 16.4kB+4.6kB/10^7 g/s. Estimate from Spring 2016 data for reduced windows is 11.5kB + 0.23kB/10^7 g/s</t>
   </si>
 </sst>
 </file>
@@ -962,7 +962,7 @@
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1112,139 +1112,142 @@
         <v>19</v>
       </c>
       <c r="B9" s="3">
-        <f>1/22</f>
-        <v>4.5454545454545456E-2</v>
+        <f>1/(340/24)</f>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="C9" s="3">
-        <f>1/22</f>
-        <v>4.5454545454545456E-2</v>
+        <f>1/(340/24)</f>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="D9" s="3">
-        <f>1/22</f>
-        <v>4.5454545454545456E-2</v>
+        <f>1/(600/36)</f>
+        <v>0.06</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="12.25" customHeight="1">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <f>B7*B9</f>
-        <v>130.67015120403209</v>
+        <v>202.92305834037927</v>
       </c>
       <c r="C10">
         <f>C7*C9</f>
-        <v>555.34814261713643</v>
+        <v>862.42299794661187</v>
       </c>
       <c r="D10">
         <f>D7*D9</f>
-        <v>1393.8149461763423</v>
+        <v>1839.8357289527719</v>
       </c>
       <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
         <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:1024" ht="12.25" customHeight="1">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3">
+        <f>(16.1+4.6*1)*1000</f>
+        <v>20700.000000000004</v>
+      </c>
+      <c r="C11" s="3">
+        <f>(11.5+2.3*2)*1000</f>
+        <v>16100.000000000002</v>
+      </c>
+      <c r="D11" s="3">
+        <f>(11.5+2.3*5)*1000</f>
+        <v>23000</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3">
-        <v>18000</v>
-      </c>
-      <c r="C11" s="3">
-        <v>18000</v>
-      </c>
-      <c r="D11" s="3">
-        <v>18000</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:1024" ht="12.25" customHeight="1">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <f>B4*B11/1000000</f>
-        <v>540</v>
+        <v>621.00000000000011</v>
       </c>
       <c r="C12">
         <f>C4*C11/1000000</f>
-        <v>900</v>
+        <v>805.00000000000011</v>
       </c>
       <c r="D12">
         <f>D4*D11/1000000</f>
-        <v>1800</v>
+        <v>2300</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:1024" ht="12.25" customHeight="1">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5">
         <f>B8*B11</f>
-        <v>1631842299794661</v>
+        <v>1876618644763860.2</v>
       </c>
       <c r="C13" s="5">
         <f>C8*C11</f>
-        <v>6935329774127309</v>
+        <v>6203267186858316</v>
       </c>
       <c r="D13" s="5">
         <f>D8*D11</f>
-        <v>1.7406317864476384E+16</v>
+        <v>2.2241406160164268E+16</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:1024">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <f>B13/1000000000000</f>
-        <v>1631.8422997946609</v>
+        <v>1876.6186447638602</v>
       </c>
       <c r="C14">
         <f>C13/1000000000000</f>
-        <v>6935.3297741273091</v>
+        <v>6203.2671868583157</v>
       </c>
       <c r="D14">
         <f>D13/1000000000000</f>
-        <v>17406.317864476383</v>
+        <v>22241.406160164268</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:1024">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3">
         <v>0.05</v>
@@ -1256,12 +1259,12 @@
         <v>0.05</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -1273,12 +1276,12 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -1290,59 +1293,59 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <f>B15*B17*B10</f>
-        <v>13.067015120403211</v>
+        <v>20.292305834037929</v>
       </c>
       <c r="C18">
         <f>C15*C17*C10</f>
-        <v>55.534814261713649</v>
+        <v>86.242299794661193</v>
       </c>
       <c r="D18">
         <f>D15*D17*D10</f>
-        <v>139.38149461763425</v>
+        <v>183.98357289527721</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <f>B16*B10</f>
-        <v>261.34030240806419</v>
+        <v>405.84611668075854</v>
       </c>
       <c r="C19">
         <f>C16*C10</f>
-        <v>1110.6962852342729</v>
+        <v>1724.8459958932237</v>
       </c>
       <c r="D19">
         <f>D16*D10</f>
-        <v>2787.6298923526847</v>
+        <v>3679.6714579055438</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3">
         <v>0.1</v>
@@ -1354,12 +1357,12 @@
         <v>0.1</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3">
         <v>0.1</v>
@@ -1371,12 +1374,12 @@
         <v>0.1</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3">
         <v>5</v>
@@ -1388,35 +1391,35 @@
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <f>B20*B10</f>
-        <v>13.067015120403211</v>
+        <v>20.292305834037929</v>
       </c>
       <c r="C23">
         <f>C20*C10</f>
-        <v>55.534814261713649</v>
+        <v>86.242299794661193</v>
       </c>
       <c r="D23">
         <f>D20*D10</f>
-        <v>139.38149461763425</v>
+        <v>183.98357289527721</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -1428,75 +1431,75 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25">
         <f>B22*B23*B24</f>
-        <v>130.67015120403209</v>
+        <v>202.9230583403793</v>
       </c>
       <c r="C25">
         <f>C22*C23*C24</f>
-        <v>555.34814261713655</v>
+        <v>862.42299794661199</v>
       </c>
       <c r="D25">
         <f>D22*D23*D24</f>
-        <v>1393.8149461763423</v>
+        <v>1839.8357289527721</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26">
         <f>B50*B21</f>
-        <v>1.0349075975359343</v>
+        <v>1.1901437371663246</v>
       </c>
       <c r="C26">
         <f>C50*C21</f>
-        <v>4.3983572895277216</v>
+        <v>3.9340862422997951</v>
       </c>
       <c r="D26">
         <f>D50*D21</f>
-        <v>11.039014373716633</v>
+        <v>14.105407255304584</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27">
         <f>B26*B22*B24*$G2/1000000000</f>
-        <v>0.32659199999999999</v>
+        <v>0.37558080000000005</v>
       </c>
       <c r="C27">
         <f>C26*C22*C24*$G2/1000000000</f>
-        <v>1.3880160000000006</v>
+        <v>1.2415032000000001</v>
       </c>
       <c r="D27">
         <f>D26*D22*D24*$G2/1000000000</f>
-        <v>3.4836480000000001</v>
+        <v>4.4513279999999993</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" s="3">
         <f>1/14.04+1/11.4</f>
@@ -1513,7 +1516,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" s="3">
         <f>1/22</f>
@@ -1530,50 +1533,50 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30">
         <f>B28/B9</f>
-        <v>3.4967761283550751</v>
+        <v>2.2517119008347075</v>
       </c>
       <c r="C30">
         <f>C28/C9</f>
-        <v>3.4967761283550751</v>
+        <v>2.2517119008347075</v>
       </c>
       <c r="D30">
         <f>D28/D9</f>
-        <v>3.4967761283550751</v>
+        <v>2.6490728245114208</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31">
         <f>B29/B9</f>
-        <v>1</v>
+        <v>0.64393939393939392</v>
       </c>
       <c r="C31">
         <f>C29/C9</f>
-        <v>1</v>
+        <v>0.64393939393939392</v>
       </c>
       <c r="D31">
         <f>D29/D9</f>
-        <v>1</v>
+        <v>0.75757575757575768</v>
       </c>
       <c r="F31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" s="3">
         <v>2</v>
@@ -1585,12 +1588,12 @@
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:1024">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B33">
         <v>18000</v>
@@ -1602,15 +1605,15 @@
         <v>18000</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:1024">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="3">
         <v>2</v>
@@ -1622,12 +1625,12 @@
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:1024">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35">
         <f>B7*B32*B34</f>
@@ -1645,35 +1648,35 @@
         <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:1024">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36">
         <f>B32*B10*(B30+B31)*B34</f>
-        <v>2350.3776664913585</v>
+        <v>2350.3776664913589</v>
       </c>
       <c r="C36">
         <f>C32*C10*(C30+C31)*C34</f>
-        <v>9989.1050825882739</v>
+        <v>9989.1050825882758</v>
       </c>
       <c r="D36">
         <f>D32*D10*(D30+D31)*D34</f>
-        <v>25070.695109241158</v>
+        <v>25070.695109241165</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:1024">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B37">
         <f>B33*B48</f>
@@ -1688,15 +1691,15 @@
         <v>3600</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:1024">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B38">
         <f>B35*B37/1000000</f>
@@ -1711,12 +1714,12 @@
         <v>441.56057494866525</v>
       </c>
       <c r="E38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:1024">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B39">
         <f>B38*$G2/1000000000</f>
@@ -1731,12 +1734,12 @@
         <v>13.934591999999999</v>
       </c>
       <c r="E39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:1024">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" s="3">
         <v>0.1</v>
@@ -1748,12 +1751,12 @@
         <v>0.1</v>
       </c>
       <c r="F40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:1024">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" s="3">
         <v>10</v>
@@ -1765,83 +1768,83 @@
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:1024">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42">
         <f>B40*B10*B41</f>
-        <v>130.67015120403209</v>
+        <v>202.9230583403793</v>
       </c>
       <c r="C42">
         <f>C40*C10*C41</f>
-        <v>555.34814261713655</v>
+        <v>862.42299794661199</v>
       </c>
       <c r="D42">
         <f>D40*D10*D41</f>
-        <v>1393.8149461763423</v>
+        <v>1839.8357289527721</v>
       </c>
       <c r="E42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F42" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:1024" s="7" customFormat="1">
       <c r="A43" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B43" s="8">
         <f>B18+B19+B25+B36+B42</f>
-        <v>2886.1252864278899</v>
+        <v>3182.362205686914</v>
       </c>
       <c r="C43" s="8">
         <f>C18+C19+C25+C36+C42</f>
-        <v>12266.032467318533</v>
+        <v>13525.039374169386</v>
       </c>
       <c r="D43" s="8">
         <f>D18+D19+D25+D36+D42</f>
-        <v>30785.336388564163</v>
+        <v>32614.021597947532</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AMI43"/>
       <c r="AMJ43"/>
     </row>
     <row r="44" spans="1:1024">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44">
         <f>B43-B36</f>
-        <v>535.74761993653146</v>
+        <v>831.98453919555504</v>
       </c>
       <c r="C44">
         <f>C43-C36</f>
-        <v>2276.9273847302593</v>
+        <v>3535.9342915811103</v>
       </c>
       <c r="D44">
         <f>D43-D36</f>
-        <v>5714.6412793230047</v>
+        <v>7543.3264887063669</v>
       </c>
       <c r="E44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:1024">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="3">
         <v>100</v>
@@ -1853,15 +1856,15 @@
         <v>100</v>
       </c>
       <c r="E45" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:1024">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" s="3">
         <v>3</v>
@@ -1873,32 +1876,32 @@
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:1024">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47">
         <f>B7*B11/B45/1000000</f>
-        <v>0.51745379876796715</v>
+        <v>0.5950718685831623</v>
       </c>
       <c r="C47">
         <f>C7*C11/C45/1000000</f>
-        <v>2.1991786447638604</v>
+        <v>1.9670431211498975</v>
       </c>
       <c r="D47">
         <f>D7*D11/D45/1000000</f>
-        <v>5.5195071868583154</v>
+        <v>7.0527036276522921</v>
       </c>
     </row>
     <row r="48" spans="1:1024">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="3">
         <v>0.2</v>
@@ -1910,288 +1913,288 @@
         <v>0.2</v>
       </c>
       <c r="F48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49">
         <f>B48*B11</f>
-        <v>3600</v>
+        <v>4140.0000000000009</v>
       </c>
       <c r="C49">
         <f>C48*C11</f>
-        <v>3600</v>
+        <v>3220.0000000000005</v>
       </c>
       <c r="D49">
         <f>D48*D11</f>
-        <v>3600</v>
+        <v>4600</v>
       </c>
       <c r="E49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B50">
         <f>B7*B49/1000000</f>
-        <v>10.349075975359343</v>
+        <v>11.901437371663246</v>
       </c>
       <c r="C50">
         <f>C7*C49/1000000</f>
-        <v>43.983572895277213</v>
+        <v>39.340862422997951</v>
       </c>
       <c r="D50">
         <f>D7*D49/1000000</f>
-        <v>110.39014373716631</v>
+        <v>141.05407255304584</v>
       </c>
       <c r="E50" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B51">
         <f>B16*B50*365.25*24*60*60/1000000000</f>
-        <v>0.65318399999999999</v>
+        <v>0.75116159999999998</v>
       </c>
       <c r="C51">
         <f>C16*C50*365.25*24*60*60/1000000000</f>
-        <v>2.7760320000000003</v>
+        <v>2.4830064000000003</v>
       </c>
       <c r="D51">
         <f>D16*D50*365.25*24*60*60/1000000000</f>
-        <v>6.9672959999999984</v>
+        <v>8.9026559999999986</v>
       </c>
       <c r="E51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B52">
         <f>B15*B7*B49/1000000</f>
-        <v>0.51745379876796715</v>
+        <v>0.5950718685831623</v>
       </c>
       <c r="C52">
         <f>C15*C7*C49/1000000</f>
-        <v>2.1991786447638604</v>
+        <v>1.9670431211498975</v>
       </c>
       <c r="D52">
         <f>D15*D7*D49/1000000</f>
-        <v>5.5195071868583163</v>
+        <v>7.052703627652293</v>
       </c>
       <c r="E52" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B53">
         <f>B17*B52*365.25*24*60*60/1000000000</f>
-        <v>3.2659199999999999E-2</v>
+        <v>3.7558080000000008E-2</v>
       </c>
       <c r="C53">
         <f>C17*C52*365.25*24*60*60/1000000000</f>
-        <v>0.1388016</v>
+        <v>0.12415032000000001</v>
       </c>
       <c r="D53">
         <f>D17*D52*365.25*24*60*60/1000000000</f>
-        <v>0.34836479999999997</v>
+        <v>0.4451328</v>
       </c>
       <c r="E53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54">
         <f>B7*(B49+B11)/(B45*1000000)</f>
-        <v>0.62094455852156061</v>
+        <v>0.71408624229979467</v>
       </c>
       <c r="C54">
         <f>C7*(C49+C11)/(C45*1000000)</f>
-        <v>2.6390143737166323</v>
+        <v>2.3604517453798772</v>
       </c>
       <c r="D54">
         <f>D7*(D49+D11)/(D45*1000000)</f>
-        <v>6.6234086242299783</v>
+        <v>8.4632443531827501</v>
       </c>
       <c r="E54" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F54" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B55">
         <f>B16*B54</f>
-        <v>1.2418891170431212</v>
+        <v>1.4281724845995893</v>
       </c>
       <c r="C55">
         <f>C16*C54</f>
-        <v>5.2780287474332646</v>
+        <v>4.7209034907597545</v>
       </c>
       <c r="D55">
         <f>D16*D54</f>
-        <v>13.246817248459957</v>
+        <v>16.9264887063655</v>
       </c>
       <c r="E55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B56">
         <f>B15*B54</f>
-        <v>3.104722792607803E-2</v>
+        <v>3.5704312114989735E-2</v>
       </c>
       <c r="C56">
         <f>C15*C54</f>
-        <v>0.13195071868583161</v>
+        <v>0.11802258726899387</v>
       </c>
       <c r="D56">
         <f>D15*D54</f>
-        <v>0.33117043121149892</v>
+        <v>0.42316221765913753</v>
       </c>
       <c r="E56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57">
         <f>B17*B56</f>
-        <v>6.2094455852156061E-2</v>
+        <v>7.140862422997947E-2</v>
       </c>
       <c r="C57">
         <f>C17*C56</f>
-        <v>0.26390143737166322</v>
+        <v>0.23604517453798773</v>
       </c>
       <c r="D57">
         <f>D17*D56</f>
-        <v>0.66234086242299783</v>
+        <v>0.84632443531827506</v>
       </c>
       <c r="E57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B58">
         <f>B7*B49/(10*1000000)</f>
-        <v>1.0349075975359343</v>
+        <v>1.1901437371663246</v>
       </c>
       <c r="C58">
         <f>C7*C49/(10*1000000)</f>
-        <v>4.3983572895277208</v>
+        <v>3.9340862422997951</v>
       </c>
       <c r="D58">
         <f>D7*D49/(10*1000000)</f>
-        <v>11.039014373716631</v>
+        <v>14.105407255304584</v>
       </c>
       <c r="E58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F58" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B59">
         <f>B22*B58*B20</f>
-        <v>0.51745379876796715</v>
+        <v>0.5950718685831623</v>
       </c>
       <c r="C59">
         <f>C22*C58*C20</f>
-        <v>2.1991786447638604</v>
+        <v>1.9670431211498975</v>
       </c>
       <c r="D59">
         <f>D22*D58*D20</f>
-        <v>5.5195071868583163</v>
+        <v>7.0527036276522921</v>
       </c>
       <c r="E59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B60">
         <f>(B58+B59)*B24</f>
-        <v>3.1047227926078032</v>
+        <v>3.570431211498974</v>
       </c>
       <c r="C60">
         <f>(C58+C59)*C24</f>
-        <v>13.195071868583163</v>
+        <v>11.802258726899385</v>
       </c>
       <c r="D60">
         <f>(D58+D59)*D24</f>
-        <v>33.117043121149891</v>
+        <v>42.316221765913753</v>
       </c>
       <c r="E60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B61">
         <f>B38/B45</f>
@@ -2206,35 +2209,35 @@
         <v>4.4156057494866525</v>
       </c>
       <c r="E61" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B62">
         <f>B47+B55+B57+B60+B61</f>
-        <v>5.3401232032854216</v>
+        <v>6.079047227926079</v>
       </c>
       <c r="C62">
         <f>C47+C55+C57+C60+C61</f>
-        <v>22.69552361396304</v>
+        <v>20.485593429158115</v>
       </c>
       <c r="D62">
         <f>D47+D55+D57+D60+D61</f>
-        <v>56.961314168377811</v>
+        <v>71.557344284736487</v>
       </c>
       <c r="F62" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B63" s="3">
         <v>20</v>
@@ -2246,15 +2249,15 @@
         <v>20</v>
       </c>
       <c r="E63" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F63" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B64">
         <f>B63*B41</f>
@@ -2269,27 +2272,27 @@
         <v>200</v>
       </c>
       <c r="E64" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B65">
         <f>B14/1000+B51+B53+B27+B39</f>
-        <v>3.9506454997946605</v>
+        <v>4.3472871247638603</v>
       </c>
       <c r="C65">
         <f>C14/1000+C51+C53+C27+C39</f>
-        <v>16.790243374127311</v>
+        <v>15.603991106858317</v>
       </c>
       <c r="D65">
         <f>D14/1000+D51+D53+D27+D39</f>
-        <v>42.140218664476379</v>
+        <v>49.975114960164262</v>
       </c>
     </row>
   </sheetData>
@@ -2319,7 +2322,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12.25" customHeight="1">
       <c r="B1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2331,12 +2334,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.25" customHeight="1">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" s="3">
         <f>model!B5</f>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="3" spans="1:8" ht="12.25" customHeight="1">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3">
         <f>7*B2</f>
@@ -2384,7 +2387,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="G3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H3" s="3">
         <v>2</v>
@@ -2392,7 +2395,7 @@
     </row>
     <row r="4" spans="1:8" ht="12.25" customHeight="1">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4">
         <f>model!B6</f>
@@ -2415,7 +2418,7 @@
         <v>fraction of wall time when beam is on, either due to beam unavailable or detector not ready</v>
       </c>
       <c r="G4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H4">
         <f>24*60*60</f>
@@ -2424,7 +2427,7 @@
     </row>
     <row r="5" spans="1:8" ht="12.25" customHeight="1">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" s="4">
         <f>B3*B4*$H$4</f>
@@ -2447,7 +2450,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="G5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H5">
         <v>365.25</v>
@@ -2455,7 +2458,7 @@
     </row>
     <row r="6" spans="1:8" ht="12.25" customHeight="1">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6">
         <v>2000</v>
@@ -2473,7 +2476,7 @@
         <v>20000</v>
       </c>
       <c r="G6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H6">
         <v>10000</v>
@@ -2481,7 +2484,7 @@
     </row>
     <row r="7" spans="1:8" ht="12.25" customHeight="1">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" s="4">
         <f>B5*B6</f>
@@ -2504,7 +2507,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="G7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H7">
         <f>model!$B32</f>
@@ -2518,28 +2521,28 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H8">
         <f>model!$B11</f>
-        <v>18000</v>
+        <v>20700.000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="12.25" customHeight="1">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9">
         <f>model!B9</f>
-        <v>4.5454545454545456E-2</v>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="C9">
         <f>model!C9</f>
-        <v>4.5454545454545456E-2</v>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="D9">
         <f>model!D9</f>
-        <v>4.5454545454545456E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E9" t="str">
         <f>model!E9</f>
@@ -2547,10 +2550,10 @@
       </c>
       <c r="F9" t="str">
         <f>model!F9</f>
-        <v>Time to reconstruct a single event on a 2.8 GHz Nehalem machine, per thread, from Simon's email of 1/31/2011</v>
+        <v>Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H9">
         <f>model!$B48</f>
@@ -2559,19 +2562,19 @@
     </row>
     <row r="10" spans="1:8" ht="12.25" customHeight="1">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B10">
         <f>B7*B9/$H$4/$H$5</f>
-        <v>8.7113434136021404</v>
+        <v>13.528203889358618</v>
       </c>
       <c r="C10">
         <f>C7*C9/$H$4/$H$5</f>
-        <v>222.13925704685457</v>
+        <v>344.96919917864477</v>
       </c>
       <c r="D10">
         <f>D7*D9/$H$4/$H$5</f>
-        <v>278.76298923526849</v>
+        <v>367.96714579055441</v>
       </c>
       <c r="E10" t="e">
         <f>E7*E9/$H$4/$H$5</f>
@@ -2584,19 +2587,19 @@
     </row>
     <row r="11" spans="1:8" ht="12.25" customHeight="1">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B11">
         <f>B7*B9/$H$4/$H$6</f>
-        <v>0.31818181818181818</v>
+        <v>0.49411764705882349</v>
       </c>
       <c r="C11">
         <f>C7*C9/$H$4/$H$6</f>
-        <v>8.1136363636363633</v>
+        <v>12.6</v>
       </c>
       <c r="D11">
         <f>D7*D9/$H$4/$H$6</f>
-        <v>10.181818181818182</v>
+        <v>13.44</v>
       </c>
       <c r="E11" t="e">
         <f>E7*E9/$H$4/$H$6</f>
@@ -2609,7 +2612,7 @@
     </row>
     <row r="13" spans="1:8" ht="12.25" customHeight="1">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13">
         <f>model!B28</f>
@@ -2634,19 +2637,19 @@
     </row>
     <row r="14" spans="1:8" ht="12.25" customHeight="1">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B14">
         <f>B9</f>
-        <v>4.5454545454545456E-2</v>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="C14">
         <f>C9</f>
-        <v>4.5454545454545456E-2</v>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="D14">
         <f>D9</f>
-        <v>4.5454545454545456E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E14" t="str">
         <f>E9</f>
@@ -2654,24 +2657,24 @@
       </c>
       <c r="F14" t="str">
         <f>F9</f>
-        <v>Time to reconstruct a single event on a 2.8 GHz Nehalem machine, per thread, from Simon's email of 1/31/2011</v>
+        <v>Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.25" customHeight="1">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B15">
         <f>B7*$H$7*(B14+B13)/$H$4/$H$6</f>
-        <v>2.8615848089532303</v>
+        <v>3.2134564667072407</v>
       </c>
       <c r="C15">
         <f>C7*$H$7*(C14+C13)/$H$4/$H$6</f>
-        <v>72.970412628307358</v>
+        <v>81.943139901034641</v>
       </c>
       <c r="D15">
         <f>D7*$H$7*(D14+D13)/$H$4/$H$6</f>
-        <v>91.57071388650337</v>
+        <v>98.087077522866991</v>
       </c>
       <c r="E15" t="e">
         <f>E7*$H$7*(E14+E13)/$H$4/$H$6</f>
@@ -2684,19 +2687,19 @@
     </row>
     <row r="17" spans="1:6" ht="12.25" customHeight="1">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17">
         <f>B11+B15</f>
-        <v>3.1797666271350487</v>
+        <v>3.7075741137660643</v>
       </c>
       <c r="C17">
         <f>C11+C15</f>
-        <v>81.084048991943718</v>
+        <v>94.543139901034635</v>
       </c>
       <c r="D17">
         <f>D11+D15</f>
-        <v>101.75253206832156</v>
+        <v>111.52707752286699</v>
       </c>
       <c r="E17" t="e">
         <f>E11+E15</f>
@@ -2709,19 +2712,19 @@
     </row>
     <row r="23" spans="1:6" ht="12.25" customHeight="1">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23">
         <f>B7*$H8</f>
-        <v>108864000000000</v>
+        <v>125193600000000.02</v>
       </c>
       <c r="C23">
         <f>C7*$H8</f>
-        <v>2776032000000000</v>
+        <v>3192436800000000.5</v>
       </c>
       <c r="D23">
         <f>D7*$H8</f>
-        <v>3483648000000000</v>
+        <v>4006195200000000.5</v>
       </c>
       <c r="E23" t="e">
         <f>E7*$H8</f>
@@ -2734,19 +2737,19 @@
     </row>
     <row r="24" spans="1:6" ht="12.25" customHeight="1">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B24">
         <f>B23/1000000000000000</f>
-        <v>0.108864</v>
+        <v>0.12519360000000002</v>
       </c>
       <c r="C24">
         <f>C23/1000000000000000</f>
-        <v>2.7760319999999998</v>
+        <v>3.1924368000000003</v>
       </c>
       <c r="D24">
         <f>D23/1000000000000000</f>
-        <v>3.4836480000000001</v>
+        <v>4.0061952000000005</v>
       </c>
       <c r="E24" t="e">
         <f>E23/1000000000000000</f>
@@ -2759,19 +2762,19 @@
     </row>
     <row r="25" spans="1:6" ht="12.25" customHeight="1">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25">
         <f>B24*$H9</f>
-        <v>2.1772800000000002E-2</v>
+        <v>2.5038720000000004E-2</v>
       </c>
       <c r="C25">
         <f>C24*$H9</f>
-        <v>0.55520639999999999</v>
+        <v>0.63848736000000006</v>
       </c>
       <c r="D25">
         <f>D24*$H9</f>
-        <v>0.69672960000000006</v>
+        <v>0.80123904000000012</v>
       </c>
       <c r="E25" t="e">
         <f>E24*$H9</f>
@@ -2784,19 +2787,19 @@
     </row>
     <row r="26" spans="1:6" ht="12.25" customHeight="1">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B26">
         <f>B24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>0.25256448000000004</v>
+        <v>0.2904491520000001</v>
       </c>
       <c r="C26">
         <f>C24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>6.4403942400000007</v>
+        <v>7.4064533760000018</v>
       </c>
       <c r="D26">
         <f>D24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>8.0820633600000011</v>
+        <v>9.2943728640000032</v>
       </c>
       <c r="E26" t="e">
         <f>E24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>

</xml_diff>

<commit_message>
Fix wait time page, use old values.
</commit_message>
<xml_diff>
--- a/computing_model_2016-11.xlsx
+++ b/computing_model_2016-11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,495 +15,480 @@
     <definedName function="false" hidden="false" name="Pass1CPUs" vbProcedure="false">model!$B$10</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="156">
-  <si>
-    <t xml:space="preserve">GlueX Computing Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fy17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fy18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">event rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">events/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw data rate out of the counting room when beam is on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annual running</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amount of running in a year, fy17: 35+67 days, fy18: 42+10+21 days (see Eugene’s talk, Oct. ‘16 Collab. Mtg.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">running efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fraction of wall time when beam is on, either due to beam unavailable or detector not ready</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effective event rate (per second)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event rate averaged over time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effective event rate (per year)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">events/year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPU time per event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPU-s/event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single Pass 1 CPU needed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPU's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of threads to keep up with the raw event rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw event size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size of a single raw event. Actual Spring 2016 data is 16.4kB+4.6kB/10^7 g/s. Estimate from Spring 2016 data for reduced windows is 11.5kB + 0.23kB/10^7 g/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw instantaneous storage rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MB/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data rate when beam is on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw effective storage rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bytes/year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average data volume rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TB/year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass 0 event fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fraction of events from raw data stream to perform calibrations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass 1 repetition factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of times event reconstruction will be repeated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass 0 repetition factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of times calibration will be repeated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass 0 CPU need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of threads of calibration to keep up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass 1 CPU need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of threads of reconstruction to keep up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stream/pass-1 CPU ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of CPU time required for a skim stream to that needed for reconstruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stream output to input size ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of data volume output for a stream to that of input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stream multiplicity factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of streams to be produced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single stream CPU need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of threads for one stream to keep up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stream repetition factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of times streaming will be repeated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stream CPU need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of threads for streaming to keep up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single stream output data rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total stream output data rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB/year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC CPU time per event, generation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC CPU time per event, reconstruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC CPU ratio per event, generation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of CPU time required for generating a Monte Carlo event to that needed for reconstruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC CPU ratio per event, reconstruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of CPU time to reconstruct Monte Carlo events to that to reconstruct real data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC/raw data event rate ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of number of Monte Carlo events needed to number of raw data events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC event size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size of a single generated Monte Carlo event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC multiplicity factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of times MC data will need to be generated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC effective event rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">event rate averaged over time of MC event generation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC CPU need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numbers of threads needed for generating Monte Carlo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC pass 1 output event size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size of a single reconstructed Monte Carlo event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC effective data rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analysis/pass-1 CPU ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of CPU time required for performing a physics analysis to that needed for reconstruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analysis multiplicity factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of analyses to be conducted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analysis CPU need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of threads needed for analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total CPU need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total number  of threads needed for all activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total CPU need exclusive of MC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total number of threads needed for all activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data rate, tape to cache disk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average rate from tape library to cache disk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data rate, cache disk to local disk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average rate from cache disk to local farm node disk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw data recording tape need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass 1 output to input size ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of output event size to input event size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass1 processed event size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reconstructed event size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single pass 1 output data rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data rate for a single pass 1 output stream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total pass 1 output data rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data rate for all pass 1 output streams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single pass 0 output data rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total pass 0 output data rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data rate for all pass 0 output streams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single pass 1 tape need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to support pass 1, one iteration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass 1 tape need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to support pass 1, all iterations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single pass 0 tape need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to support pass 0, one iteration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass 0 tape need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to support pass 0, all iterations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single stream input tape need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to support input for streaming, one iteration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single set of stream output tape need (all streams)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to support output for streaming, one iteration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total stream tape need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to support streaming, all iterations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC tape drive need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of tape drives needed to archive reconstructed MC data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total tape drive need</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total number of tape drives needed for all activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disk usage per analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permanent disk space used by an analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disk usage total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permanent disk space used by all analyses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total output rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fy15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fy16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fy19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weeks of running</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Days of running</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Days of Running per PAC Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Running efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seconds per day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Running time (s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Days per year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trigger rate (Hz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of cores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio of Monte Carlo events to data events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">event size (bytes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reconstruction time per event per core (s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratio of size of DST to Raw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reconstruction time, single core (y)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reconstruction time (d)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monte Carlo generation time per event per core</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monte Carlo reconstruction time per event per core</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monte Carlo time, gen. + recon. (d)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reconstruction time + MC time (d)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw data volume (bytes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raw data volume (PB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DST data volume, real data, recon. (PB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total data to tape (PB)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
+  <si>
+    <t>GlueX Computing Model</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>fy17</t>
+  </si>
+  <si>
+    <t>fy18</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>event rate</t>
+  </si>
+  <si>
+    <t>events/s</t>
+  </si>
+  <si>
+    <t>raw data rate out of the counting room when beam is on</t>
+  </si>
+  <si>
+    <t>annual running</t>
+  </si>
+  <si>
+    <t>weeks</t>
+  </si>
+  <si>
+    <t>amount of running in a year, fy17: 35+67 days, fy18: 42+10+21 days (see Eugene’s talk, Oct. ‘16 Collab. Mtg.)</t>
+  </si>
+  <si>
+    <t>running efficiency</t>
+  </si>
+  <si>
+    <t>fraction of wall time when beam is on, either due to beam unavailable or detector not ready</t>
+  </si>
+  <si>
+    <t>effective event rate (per second)</t>
+  </si>
+  <si>
+    <t>Event rate averaged over time</t>
+  </si>
+  <si>
+    <t>effective event rate (per year)</t>
+  </si>
+  <si>
+    <t>events/year</t>
+  </si>
+  <si>
+    <t>CPU time per event</t>
+  </si>
+  <si>
+    <t>CPU-s/event</t>
+  </si>
+  <si>
+    <t>Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</t>
+  </si>
+  <si>
+    <t>single Pass 1 CPU needed</t>
+  </si>
+  <si>
+    <t>CPU's</t>
+  </si>
+  <si>
+    <t>number of threads to keep up with the raw event rate</t>
+  </si>
+  <si>
+    <t>raw event size</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>size of a single raw event. Actual Spring 2016 data is 16.4kB+4.6kB/10^7 g/s. Estimate from Spring 2016 data for reduced windows is 11.5kB + 0.23kB/10^7 g/s</t>
+  </si>
+  <si>
+    <t>raw instantaneous storage rate</t>
+  </si>
+  <si>
+    <t>MB/s</t>
+  </si>
+  <si>
+    <t>data rate when beam is on</t>
+  </si>
+  <si>
+    <t>raw effective storage rate</t>
+  </si>
+  <si>
+    <t>bytes/year</t>
+  </si>
+  <si>
+    <t>average data volume rate</t>
+  </si>
+  <si>
+    <t>TB/year</t>
+  </si>
+  <si>
+    <t>pass 0 event fraction</t>
+  </si>
+  <si>
+    <t>fraction of events from raw data stream to perform calibrations</t>
+  </si>
+  <si>
+    <t>pass 1 repetition factor</t>
+  </si>
+  <si>
+    <t>number of times event reconstruction will be repeated</t>
+  </si>
+  <si>
+    <t>pass 0 repetition factor</t>
+  </si>
+  <si>
+    <t>number of times calibration will be repeated</t>
+  </si>
+  <si>
+    <t>pass 0 CPU need</t>
+  </si>
+  <si>
+    <t>number of threads of calibration to keep up</t>
+  </si>
+  <si>
+    <t>pass 1 CPU need</t>
+  </si>
+  <si>
+    <t>number of threads of reconstruction to keep up</t>
+  </si>
+  <si>
+    <t>stream/pass-1 CPU ratio</t>
+  </si>
+  <si>
+    <t>ratio of CPU time required for a skim stream to that needed for reconstruction</t>
+  </si>
+  <si>
+    <t>stream output to input size ratio</t>
+  </si>
+  <si>
+    <t>ratio of data volume output for a stream to that of input</t>
+  </si>
+  <si>
+    <t>stream multiplicity factor</t>
+  </si>
+  <si>
+    <t>number of streams to be produced</t>
+  </si>
+  <si>
+    <t>single stream CPU need</t>
+  </si>
+  <si>
+    <t>number of threads for one stream to keep up</t>
+  </si>
+  <si>
+    <t>stream repetition factor</t>
+  </si>
+  <si>
+    <t>number of times streaming will be repeated</t>
+  </si>
+  <si>
+    <t>stream CPU need</t>
+  </si>
+  <si>
+    <t>number of threads for streaming to keep up</t>
+  </si>
+  <si>
+    <t>single stream output data rate</t>
+  </si>
+  <si>
+    <t>total stream output data rate</t>
+  </si>
+  <si>
+    <t>PB/year</t>
+  </si>
+  <si>
+    <t>MC CPU time per event, generation</t>
+  </si>
+  <si>
+    <t>MC CPU time per event, reconstruction</t>
+  </si>
+  <si>
+    <t>MC CPU ratio per event, generation</t>
+  </si>
+  <si>
+    <t>ratio of CPU time required for generating a Monte Carlo event to that needed for reconstruction</t>
+  </si>
+  <si>
+    <t>MC CPU ratio per event, reconstruction</t>
+  </si>
+  <si>
+    <t>ratio of CPU time to reconstruct Monte Carlo events to that to reconstruct real data</t>
+  </si>
+  <si>
+    <t>MC/raw data event rate ratio</t>
+  </si>
+  <si>
+    <t>ratio of number of Monte Carlo events needed to number of raw data events</t>
+  </si>
+  <si>
+    <t>MC event size</t>
+  </si>
+  <si>
+    <t>size of a single generated Monte Carlo event</t>
+  </si>
+  <si>
+    <t>MC multiplicity factor</t>
+  </si>
+  <si>
+    <t>number of times MC data will need to be generated</t>
+  </si>
+  <si>
+    <t>MC effective event rate</t>
+  </si>
+  <si>
+    <t>event rate averaged over time of MC event generation</t>
+  </si>
+  <si>
+    <t>MC CPU need</t>
+  </si>
+  <si>
+    <t>numbers of threads needed for generating Monte Carlo</t>
+  </si>
+  <si>
+    <t>MC pass 1 output event size</t>
+  </si>
+  <si>
+    <t>size of a single reconstructed Monte Carlo event</t>
+  </si>
+  <si>
+    <t>MC effective data rate</t>
+  </si>
+  <si>
+    <t>analysis/pass-1 CPU ratio</t>
+  </si>
+  <si>
+    <t>ratio of CPU time required for performing a physics analysis to that needed for reconstruction</t>
+  </si>
+  <si>
+    <t>analysis multiplicity factor</t>
+  </si>
+  <si>
+    <t>number of analyses to be conducted</t>
+  </si>
+  <si>
+    <t>analysis CPU need</t>
+  </si>
+  <si>
+    <t>number of threads needed for analysis</t>
+  </si>
+  <si>
+    <t>total CPU need</t>
+  </si>
+  <si>
+    <t>total number  of threads needed for all activities</t>
+  </si>
+  <si>
+    <t>total CPU need exclusive of MC</t>
+  </si>
+  <si>
+    <t>total number of threads needed for all activities</t>
+  </si>
+  <si>
+    <t>data rate, tape to cache disk</t>
+  </si>
+  <si>
+    <t>average rate from tape library to cache disk</t>
+  </si>
+  <si>
+    <t>data rate, cache disk to local disk</t>
+  </si>
+  <si>
+    <t>average rate from cache disk to local farm node disk</t>
+  </si>
+  <si>
+    <t>raw data recording tape need</t>
+  </si>
+  <si>
+    <t>Pass 1 output to input size ratio</t>
+  </si>
+  <si>
+    <t>ratio of output event size to input event size</t>
+  </si>
+  <si>
+    <t>pass1 processed event size</t>
+  </si>
+  <si>
+    <t>reconstructed event size</t>
+  </si>
+  <si>
+    <t>Single pass 1 output data rate</t>
+  </si>
+  <si>
+    <t>data rate for a single pass 1 output stream</t>
+  </si>
+  <si>
+    <t>total pass 1 output data rate</t>
+  </si>
+  <si>
+    <t>data rate for all pass 1 output streams</t>
+  </si>
+  <si>
+    <t>Single pass 0 output data rate</t>
+  </si>
+  <si>
+    <t>total pass 0 output data rate</t>
+  </si>
+  <si>
+    <t>data rate for all pass 0 output streams</t>
+  </si>
+  <si>
+    <t>single pass 1 tape need</t>
+  </si>
+  <si>
+    <t>drives</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to support pass 1, one iteration</t>
+  </si>
+  <si>
+    <t>Pass 1 tape need</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to support pass 1, all iterations</t>
+  </si>
+  <si>
+    <t>single pass 0 tape need</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to support pass 0, one iteration</t>
+  </si>
+  <si>
+    <t>Pass 0 tape need</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to support pass 0, all iterations</t>
+  </si>
+  <si>
+    <t>single stream input tape need</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to support input for streaming, one iteration</t>
+  </si>
+  <si>
+    <t>single set of stream output tape need (all streams)</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to support output for streaming, one iteration</t>
+  </si>
+  <si>
+    <t>total stream tape need</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to support streaming, all iterations</t>
+  </si>
+  <si>
+    <t>MC tape drive need</t>
+  </si>
+  <si>
+    <t>number of tape drives needed to archive reconstructed MC data</t>
+  </si>
+  <si>
+    <t>total tape drive need</t>
+  </si>
+  <si>
+    <t>total number of tape drives needed for all activities</t>
+  </si>
+  <si>
+    <t>disk usage per analysis</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>permanent disk space used by an analysis</t>
+  </si>
+  <si>
+    <t>disk usage total</t>
+  </si>
+  <si>
+    <t>permanent disk space used by all analyses</t>
+  </si>
+  <si>
+    <t>total output rate</t>
+  </si>
+  <si>
+    <t>Weeks of running</t>
+  </si>
+  <si>
+    <t>Days of running</t>
+  </si>
+  <si>
+    <t>Days of Running per PAC Day</t>
+  </si>
+  <si>
+    <t>Running efficiency</t>
+  </si>
+  <si>
+    <t>Seconds per day</t>
+  </si>
+  <si>
+    <t>Running time (s)</t>
+  </si>
+  <si>
+    <t>Days per year</t>
+  </si>
+  <si>
+    <t>Trigger rate (Hz)</t>
+  </si>
+  <si>
+    <t>Number of cores</t>
+  </si>
+  <si>
+    <t>Number of events</t>
+  </si>
+  <si>
+    <t>Ratio of Monte Carlo events to data events</t>
+  </si>
+  <si>
+    <t>event size (bytes)</t>
+  </si>
+  <si>
+    <t>Reconstruction time per event per core (s)</t>
+  </si>
+  <si>
+    <t>ratio of size of DST to Raw</t>
+  </si>
+  <si>
+    <t>Reconstruction time, single core (y)</t>
+  </si>
+  <si>
+    <t>Reconstruction time (d)</t>
+  </si>
+  <si>
+    <t>Monte Carlo generation time per event per core</t>
+  </si>
+  <si>
+    <t>Monte Carlo reconstruction time per event per core</t>
+  </si>
+  <si>
+    <t>Monte Carlo time, gen. + recon. (d)</t>
+  </si>
+  <si>
+    <t>Reconstruction time + MC time (d)</t>
+  </si>
+  <si>
+    <t>raw data volume (bytes)</t>
+  </si>
+  <si>
+    <t>raw data volume (PB)</t>
+  </si>
+  <si>
+    <t>DST data volume, real data, recon. (PB)</t>
+  </si>
+  <si>
+    <t>total data to tape (PB)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
     <numFmt numFmtId="167" formatCode="##0.0E+0"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -589,7 +574,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -627,10 +612,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -713,8 +694,8 @@
   </sheetPr>
   <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1833,505 +1814,293 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="1" sqref="B5:E5 B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="3" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C2" s="3" t="n">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <f aca="false">model!B5</f>
         <v>14.5714285714286</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="3" t="n">
         <f aca="false">model!C5</f>
         <v>10.4285714285714</v>
       </c>
-      <c r="E2" s="3" t="str">
-        <f aca="false">model!D5</f>
-        <v>weeks</v>
-      </c>
-      <c r="F2" s="3" t="str">
-        <f aca="false">model!E5</f>
-        <v>amount of running in a year, fy17: 35+67 days, fy18: 42+10+21 days (see Eugene’s talk, Oct. ‘16 Collab. Mtg.)</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="0" t="e">
+        <v>130</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <f aca="false">7*B2</f>
-        <v>#REF!</v>
+        <v>102</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">7*C2</f>
-        <v>102</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">7*D2</f>
         <v>73</v>
       </c>
-      <c r="E3" s="0" t="e">
-        <f aca="false">7*E2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" s="0" t="e">
-        <f aca="false">7*F2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="3" t="n">
+      <c r="D3" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="0" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <f aca="false">model!B6</f>
         <v>0.5</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <f aca="false">model!C6</f>
         <v>0.5</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>133</v>
+      </c>
       <c r="E4" s="0" t="n">
-        <f aca="false">model!D6</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="str">
-        <f aca="false">model!E6</f>
-        <v>fraction of wall time when beam is on, either due to beam unavailable or detector not ready</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="0" t="n">
         <f aca="false">24*60*60</f>
         <v>86400</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="5" t="e">
-        <f aca="false">B3*B4*$H$4</f>
-        <v>#REF!</v>
+        <v>134</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <f aca="false">B3*B4*$E$4</f>
+        <v>4406400</v>
       </c>
       <c r="C5" s="5" t="n">
-        <f aca="false">C3*C4*$H$4</f>
-        <v>4406400</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <f aca="false">D3*D4*$H$4</f>
+        <f aca="false">C3*C4*$E$4</f>
         <v>3153600</v>
       </c>
-      <c r="E5" s="5" t="e">
-        <f aca="false">E3*E4*$H$4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F5" s="5" t="e">
-        <f aca="false">F3*F4*$H$4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="D5" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>365.25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>20000</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>20000</v>
+      <c r="D6" s="0" t="s">
+        <v>137</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>20000</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="H6" s="0" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="5" t="e">
+        <v>138</v>
+      </c>
+      <c r="B7" s="5" t="n">
         <f aca="false">B5*B6</f>
-        <v>#REF!</v>
+        <v>88128000000</v>
       </c>
       <c r="C7" s="5" t="n">
         <f aca="false">C5*C6</f>
-        <v>88128000000</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <f aca="false">D5*D6</f>
         <v>63072000000</v>
       </c>
-      <c r="E7" s="5" t="e">
-        <f aca="false">E5*E6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F7" s="5" t="e">
-        <f aca="false">F5*F6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H7" s="0" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="D7" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="0" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="D8" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>18000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" s="0" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C9" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <f aca="false">model!B9</f>
         <v>0.0705882352941176</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="C9" s="0" t="n">
         <f aca="false">model!C9</f>
         <v>0.06</v>
       </c>
-      <c r="E9" s="0" t="str">
-        <f aca="false">model!D9</f>
-        <v>CPU-s/event</v>
-      </c>
-      <c r="F9" s="0" t="str">
-        <f aca="false">model!E9</f>
-        <v>Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="0" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
+      <c r="D9" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" s="0" t="e">
-        <f aca="false">B7*B9/$H$4/$H$5</f>
-        <v>#REF!</v>
+        <v>143</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">B7*B9/$E$4/$E$5</f>
+        <v>197.125256673511</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">C7*C9/$H$4/$H$5</f>
-        <v>197.125256673511</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">D7*D9/$H$4/$H$5</f>
+        <f aca="false">C7*C9/$E$4/$E$5</f>
         <v>119.917864476386</v>
-      </c>
-      <c r="E10" s="0" t="e">
-        <f aca="false">E7*E9/$H$4/$H$5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F10" s="0" t="e">
-        <f aca="false">F7*F9/$H$4/$H$5</f>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="0" t="e">
-        <f aca="false">B7*B9/$H$4/$H$6</f>
-        <v>#REF!</v>
+        <v>144</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">B7*B9/$E$4/$E$6</f>
+        <v>7.2</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">C7*C9/$H$4/$H$6</f>
-        <v>7.2</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">D7*D9/$H$4/$H$6</f>
+        <f aca="false">C7*C9/$E$4/$E$6</f>
         <v>4.38</v>
-      </c>
-      <c r="E11" s="0" t="e">
-        <f aca="false">E7*E9/$H$4/$H$6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F11" s="10" t="e">
-        <f aca="false">F7*F9/$H$4/$H$6</f>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="0" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C13" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="B13" s="0" t="n">
         <f aca="false">model!B28</f>
         <v>0.158944369470685</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="C13" s="0" t="n">
         <f aca="false">model!C28</f>
         <v>0.158944369470685</v>
       </c>
-      <c r="E13" s="0" t="n">
-        <f aca="false">model!D28</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <f aca="false">model!E28</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B14" s="0" t="e">
+        <v>146</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <f aca="false">B9</f>
-        <v>#REF!</v>
+        <v>0.0705882352941176</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">C9</f>
-        <v>0.0705882352941176</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <f aca="false">D9</f>
         <v>0.06</v>
-      </c>
-      <c r="E14" s="0" t="str">
-        <f aca="false">E9</f>
-        <v>CPU-s/event</v>
-      </c>
-      <c r="F14" s="0" t="str">
-        <f aca="false">F9</f>
-        <v>Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="0" t="e">
-        <f aca="false">B7*$H$7*(B14+B13)/$H$4/$H$6</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C15" s="0" t="e">
-        <f aca="false">C7*$H$7*(C14+C13)/$H$4/$H$6</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D15" s="0" t="e">
-        <f aca="false">D7*$H$7*(D14+D13)/$H$4/$H$6</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E15" s="0" t="e">
-        <f aca="false">E7*$H$7*(E14+E13)/$H$4/$H$6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F15" s="0" t="e">
-        <f aca="false">F7*$H$7*(F14+F13)/$H$4/$H$6</f>
-        <v>#VALUE!</v>
+        <v>147</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">B7*$E$7*(B14+B13)/$E$4/$E$6</f>
+        <v>46.8246513720198</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">C7*$E$7*(C14+C13)/$E$4/$E$6</f>
+        <v>31.96587794272</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="0" t="e">
+        <v>148</v>
+      </c>
+      <c r="B17" s="0" t="n">
         <f aca="false">B11+B15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C17" s="0" t="e">
+        <v>54.0246513720197</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <f aca="false">C11+C15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D17" s="0" t="e">
-        <f aca="false">D11+D15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E17" s="0" t="e">
-        <f aca="false">E11+E15</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F17" s="0" t="e">
-        <f aca="false">F11+F15</f>
-        <v>#VALUE!</v>
+        <v>36.34587794272</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23" s="0" t="e">
-        <f aca="false">B7*$H8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C23" s="0" t="e">
-        <f aca="false">C7*$H8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D23" s="0" t="e">
-        <f aca="false">D7*$H8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E23" s="0" t="e">
-        <f aca="false">E7*$H8</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F23" s="0" t="e">
-        <f aca="false">F7*$H8</f>
-        <v>#VALUE!</v>
+        <v>149</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">B7*$E8</f>
+        <v>1586304000000000</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <f aca="false">C7*$E8</f>
+        <v>1135296000000000</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="0" t="e">
-        <f aca="false">B23/1000000000000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C24" s="0" t="e">
-        <f aca="false">C23/1000000000000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D24" s="0" t="e">
-        <f aca="false">D23/1000000000000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E24" s="0" t="e">
-        <f aca="false">E23/1000000000000000</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F24" s="0" t="e">
-        <f aca="false">F23/1000000000000000</f>
-        <v>#VALUE!</v>
+        <v>150</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">B23/1E+015</f>
+        <v>1.586304</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <f aca="false">C23/1E+015</f>
+        <v>1.135296</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B25" s="0" t="e">
-        <f aca="false">B24*$H9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C25" s="0" t="e">
-        <f aca="false">C24*$H9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D25" s="0" t="e">
-        <f aca="false">D24*$H9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E25" s="0" t="e">
-        <f aca="false">E24*$H9</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F25" s="0" t="e">
-        <f aca="false">F24*$H9</f>
-        <v>#VALUE!</v>
+        <v>151</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">B24*$E9</f>
+        <v>0.3172608</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <f aca="false">C24*$E9</f>
+        <v>0.2270592</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B26" s="0" t="e">
+        <v>152</v>
+      </c>
+      <c r="B26" s="0" t="n">
         <f aca="false">B24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C26" s="0" t="e">
+        <v>3.68022528</v>
+      </c>
+      <c r="C26" s="0" t="n">
         <f aca="false">C24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D26" s="0" t="e">
-        <f aca="false">D24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E26" s="0" t="e">
-        <f aca="false">E24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F26" s="0" t="e">
-        <f aca="false">F24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>
-        <v>#VALUE!</v>
+        <v>2.63388672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use real event sizes for MC event sizes. Use real even reconstruction time for MC reconstruction time.
</commit_message>
<xml_diff>
--- a/computing_model_2016-11.xlsx
+++ b/computing_model_2016-11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" state="visible" r:id="rId2"/>
@@ -574,7 +574,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -605,6 +605,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -694,14 +698,14 @@
   </sheetPr>
   <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.9540816326531"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.63775510204082"/>
   </cols>
@@ -1161,13 +1165,13 @@
       <c r="A29" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="3" t="n">
-        <f aca="false">1/22</f>
-        <v>0.0454545454545455</v>
-      </c>
-      <c r="C29" s="3" t="n">
-        <f aca="false">1/22</f>
-        <v>0.0454545454545455</v>
+      <c r="B29" s="8" t="n">
+        <f aca="false">B9</f>
+        <v>0.0705882352941176</v>
+      </c>
+      <c r="C29" s="8" t="n">
+        <f aca="false">C9</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,11 +1199,11 @@
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">B29/B9</f>
-        <v>0.643939393939394</v>
+        <v>1</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C29/C9</f>
-        <v>0.757575757575758</v>
+        <v>1</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>64</v>
@@ -1275,11 +1279,11 @@
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">B32*B10*(B30+B31)*B34</f>
-        <v>5708.0600471933</v>
+        <v>6409.94543080353</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C32*C10*(C30+C31)*C34</f>
-        <v>8170.36045970806</v>
+        <v>8751.78040868447</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>22</v>
@@ -1386,22 +1390,22 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
+    <row r="43" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="9" t="n">
+      <c r="B43" s="10" t="n">
         <f aca="false">B18+B19+B25+B36+B42</f>
-        <v>7728.59392809679</v>
-      </c>
-      <c r="C43" s="9" t="n">
+        <v>8430.47931170702</v>
+      </c>
+      <c r="C43" s="10" t="n">
         <f aca="false">C18+C19+C25+C36+C42</f>
-        <v>10628.676681474</v>
-      </c>
-      <c r="D43" s="8" t="s">
+        <v>11210.0966304504</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="9" t="s">
         <v>85</v>
       </c>
       <c r="AMJ43" s="0"/>
@@ -1816,7 +1820,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
For simplicity, using same values for fy17 and fy18.
event rate = 50 kHz
reconstruction rate per thread = 9.8 Hz
simulation event production rate = 18 Hz

as per David's email of Oct. 31.
</commit_message>
<xml_diff>
--- a/computing_model_2016-11.xlsx
+++ b/computing_model_2016-11.xlsx
@@ -81,7 +81,7 @@
     <t>CPU-s/event</t>
   </si>
   <si>
-    <t>Oct. 2016 David benchmark gave 250Hz for 16 threads on Ivy Bridge, 340Hz for 24 threads on Haswell, 600Hz for 36 threads on Broadwell</t>
+    <t>Oct. 2016 David benchmark</t>
   </si>
   <si>
     <t>single Pass 1 CPU needed</t>
@@ -574,7 +574,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -605,10 +605,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -698,8 +694,8 @@
   </sheetPr>
   <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -747,7 +743,7 @@
         <v>50000</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -799,7 +795,7 @@
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">C4*C5/(365.25/7)*C6</f>
-        <v>9993.15537303217</v>
+        <v>4996.57768651607</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
@@ -818,7 +814,7 @@
       </c>
       <c r="C8" s="5" t="n">
         <f aca="false">C7*365*24*60*60</f>
-        <v>315144147843.942</v>
+        <v>157572073921.971</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>17</v>
@@ -832,12 +828,12 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="n">
-        <f aca="false">1/(340/24)</f>
-        <v>0.0705882352941176</v>
+        <f aca="false">1/9.8</f>
+        <v>0.102040816326531</v>
       </c>
       <c r="C9" s="3" t="n">
-        <f aca="false">1/(600/36)</f>
-        <v>0.06</v>
+        <f aca="false">1/9.8</f>
+        <v>0.102040816326531</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>19</v>
@@ -852,11 +848,11 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B7*B9</f>
-        <v>492.813141683778</v>
+        <v>712.399949712945</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">C7*C9</f>
-        <v>599.58932238193</v>
+        <v>509.854865971028</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>22</v>
@@ -894,7 +890,7 @@
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">C4*C11/1000000</f>
-        <v>2300</v>
+        <v>1150</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>28</v>
@@ -913,7 +909,7 @@
       </c>
       <c r="C13" s="6" t="n">
         <f aca="false">C8*C11</f>
-        <v>7248315400410680</v>
+        <v>3624157700205330</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>31</v>
@@ -932,7 +928,7 @@
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">C13/1000000000000</f>
-        <v>7248.31540041068</v>
+        <v>3624.15770020533</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>33</v>
@@ -989,11 +985,11 @@
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">B15*B17*B10</f>
-        <v>49.2813141683778</v>
+        <v>71.2399949712945</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">C15*C17*C10</f>
-        <v>59.958932238193</v>
+        <v>50.9854865971028</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>22</v>
@@ -1008,11 +1004,11 @@
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">B16*B10</f>
-        <v>985.626283367556</v>
+        <v>1424.79989942589</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C16*C10</f>
-        <v>1199.17864476386</v>
+        <v>1019.70973194206</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>22</v>
@@ -1070,11 +1066,11 @@
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B20*B10</f>
-        <v>49.2813141683778</v>
+        <v>71.2399949712945</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">C20*C10</f>
-        <v>59.958932238193</v>
+        <v>50.9854865971028</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>22</v>
@@ -1103,11 +1099,11 @@
       </c>
       <c r="B25" s="0" t="n">
         <f aca="false">B22*B23*B24</f>
-        <v>492.813141683778</v>
+        <v>712.399949712945</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C22*C23*C24</f>
-        <v>599.58932238193</v>
+        <v>509.854865971028</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>22</v>
@@ -1126,7 +1122,7 @@
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C50*C21</f>
-        <v>4.5968514715948</v>
+        <v>2.29842573579739</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>28</v>
@@ -1142,7 +1138,7 @@
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26*C22*C24*$F2/1000000000</f>
-        <v>1.450656</v>
+        <v>0.725327999999998</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>58</v>
@@ -1153,25 +1149,25 @@
         <v>59</v>
       </c>
       <c r="B28" s="3" t="n">
-        <f aca="false">1/14.04+1/11.4</f>
-        <v>0.158944369470685</v>
+        <f aca="false">1/18</f>
+        <v>0.0555555555555556</v>
       </c>
       <c r="C28" s="3" t="n">
-        <f aca="false">1/14.04+1/11.4</f>
-        <v>0.158944369470685</v>
+        <f aca="false">1/18</f>
+        <v>0.0555555555555556</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="0" t="n">
         <f aca="false">B9</f>
-        <v>0.0705882352941176</v>
-      </c>
-      <c r="C29" s="8" t="n">
+        <v>0.102040816326531</v>
+      </c>
+      <c r="C29" s="0" t="n">
         <f aca="false">C9</f>
-        <v>0.06</v>
+        <v>0.102040816326531</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1180,11 +1176,11 @@
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">B28/B9</f>
-        <v>2.25171190083471</v>
+        <v>0.544444444444444</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C28/C9</f>
-        <v>2.64907282451142</v>
+        <v>0.544444444444444</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>19</v>
@@ -1264,7 +1260,7 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C7*C32*C34</f>
-        <v>39972.6214921287</v>
+        <v>19986.3107460643</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>7</v>
@@ -1279,11 +1275,11 @@
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">B32*B10*(B30+B31)*B34</f>
-        <v>6409.94543080353</v>
+        <v>4401.04857822664</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C32*C10*(C30+C31)*C34</f>
-        <v>8751.78040868447</v>
+        <v>3149.77006088768</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>22</v>
@@ -1321,7 +1317,7 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C35*C37/1000000</f>
-        <v>143.901437371663</v>
+        <v>71.9507186858314</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>28</v>
@@ -1337,7 +1333,7 @@
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">C38*$F2/1000000000</f>
-        <v>4.541184</v>
+        <v>2.27059199999999</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>58</v>
@@ -1377,11 +1373,11 @@
       </c>
       <c r="B42" s="0" t="n">
         <f aca="false">B40*B10*B41</f>
-        <v>492.813141683778</v>
+        <v>712.399949712945</v>
       </c>
       <c r="C42" s="0" t="n">
         <f aca="false">C40*C10*C41</f>
-        <v>599.58932238193</v>
+        <v>509.854865971028</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>22</v>
@@ -1390,22 +1386,22 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="s">
+    <row r="43" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="10" t="n">
+      <c r="B43" s="9" t="n">
         <f aca="false">B18+B19+B25+B36+B42</f>
-        <v>8430.47931170702</v>
-      </c>
-      <c r="C43" s="10" t="n">
+        <v>7321.88837204971</v>
+      </c>
+      <c r="C43" s="9" t="n">
         <f aca="false">C18+C19+C25+C36+C42</f>
-        <v>11210.0966304504</v>
-      </c>
-      <c r="D43" s="9" t="s">
+        <v>5240.1750113689</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="8" t="s">
         <v>85</v>
       </c>
       <c r="AMJ43" s="0"/>
@@ -1416,11 +1412,11 @@
       </c>
       <c r="B44" s="0" t="n">
         <f aca="false">B43-B36</f>
-        <v>2020.53388090349</v>
+        <v>2920.83979382307</v>
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">C43-C36</f>
-        <v>2458.31622176591</v>
+        <v>2090.40495048121</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>22</v>
@@ -1473,7 +1469,7 @@
       </c>
       <c r="C47" s="0" t="n">
         <f aca="false">C7*C11/C45/1000000</f>
-        <v>2.2984257357974</v>
+        <v>1.1492128678987</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,7 +1515,7 @@
       </c>
       <c r="C50" s="0" t="n">
         <f aca="false">C7*C49/1000000</f>
-        <v>45.968514715948</v>
+        <v>22.9842573579739</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>28</v>
@@ -1538,7 +1534,7 @@
       </c>
       <c r="C51" s="0" t="n">
         <f aca="false">C16*C50*365.25*24*60*60/1000000000</f>
-        <v>2.901312</v>
+        <v>1.450656</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>58</v>
@@ -1557,7 +1553,7 @@
       </c>
       <c r="C52" s="0" t="n">
         <f aca="false">C15*C7*C49/1000000</f>
-        <v>2.2984257357974</v>
+        <v>1.1492128678987</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>28</v>
@@ -1576,7 +1572,7 @@
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">C17*C52*365.25*24*60*60/1000000000</f>
-        <v>0.1450656</v>
+        <v>0.0725327999999998</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>58</v>
@@ -1595,7 +1591,7 @@
       </c>
       <c r="C54" s="0" t="n">
         <f aca="false">C7*(C49+C11)/(C45*1000000)</f>
-        <v>2.75811088295688</v>
+        <v>1.37905544147844</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>105</v>
@@ -1614,7 +1610,7 @@
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">C16*C54</f>
-        <v>5.51622176591376</v>
+        <v>2.75811088295687</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>105</v>
@@ -1633,7 +1629,7 @@
       </c>
       <c r="C56" s="0" t="n">
         <f aca="false">C15*C54</f>
-        <v>0.137905544147844</v>
+        <v>0.0689527720739218</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>105</v>
@@ -1652,7 +1648,7 @@
       </c>
       <c r="C57" s="0" t="n">
         <f aca="false">C17*C56</f>
-        <v>0.275811088295688</v>
+        <v>0.137905544147844</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>105</v>
@@ -1671,7 +1667,7 @@
       </c>
       <c r="C58" s="0" t="n">
         <f aca="false">C7*C49/(10*1000000)</f>
-        <v>4.5968514715948</v>
+        <v>2.29842573579739</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>105</v>
@@ -1690,7 +1686,7 @@
       </c>
       <c r="C59" s="0" t="n">
         <f aca="false">C22*C58*C20</f>
-        <v>2.2984257357974</v>
+        <v>1.1492128678987</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>105</v>
@@ -1709,7 +1705,7 @@
       </c>
       <c r="C60" s="0" t="n">
         <f aca="false">(C58+C59)*C24</f>
-        <v>13.7905544147844</v>
+        <v>6.89527720739218</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>105</v>
@@ -1728,7 +1724,7 @@
       </c>
       <c r="C61" s="0" t="n">
         <f aca="false">C38/C45</f>
-        <v>1.43901437371663</v>
+        <v>0.719507186858314</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>105</v>
@@ -1747,7 +1743,7 @@
       </c>
       <c r="C62" s="0" t="n">
         <f aca="false">C47+C55+C57+C60+C61</f>
-        <v>23.3200273785079</v>
+        <v>11.6600136892539</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>122</v>
@@ -1799,7 +1795,7 @@
       </c>
       <c r="C65" s="0" t="n">
         <f aca="false">C14/1000+C51+C53+C27+C39</f>
-        <v>16.2865330004107</v>
+        <v>8.14326650020532</v>
       </c>
     </row>
   </sheetData>
@@ -1964,11 +1960,11 @@
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">model!B9</f>
-        <v>0.0705882352941176</v>
+        <v>0.102040816326531</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">model!C9</f>
-        <v>0.06</v>
+        <v>0.102040816326531</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>142</v>
@@ -1983,11 +1979,11 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B7*B9/$E$4/$E$5</f>
-        <v>197.125256673511</v>
+        <v>284.959979885178</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">C7*C9/$E$4/$E$5</f>
-        <v>119.917864476386</v>
+        <v>203.941946388412</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1996,11 +1992,11 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B7*B9/$E$4/$E$6</f>
-        <v>7.2</v>
+        <v>10.4081632653061</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">C7*C9/$E$4/$E$6</f>
-        <v>4.38</v>
+        <v>7.44897959183673</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2009,11 +2005,11 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">model!B28</f>
-        <v>0.158944369470685</v>
+        <v>0.0555555555555556</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">model!C28</f>
-        <v>0.158944369470685</v>
+        <v>0.0555555555555556</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2022,11 +2018,11 @@
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">B9</f>
-        <v>0.0705882352941176</v>
+        <v>0.102040816326531</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">C9</f>
-        <v>0.06</v>
+        <v>0.102040816326531</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2035,11 +2031,11 @@
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">B7*$E$7*(B14+B13)/$E$4/$E$6</f>
-        <v>46.8246513720198</v>
+        <v>32.1496598639456</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">C7*$E$7*(C14+C13)/$E$4/$E$6</f>
-        <v>31.96587794272</v>
+        <v>23.0090702947846</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2048,11 +2044,11 @@
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">B11+B15</f>
-        <v>54.0246513720197</v>
+        <v>42.5578231292517</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">C11+C15</f>
-        <v>36.34587794272</v>
+        <v>30.4580498866213</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Put in factor of 2 for G3 -> G4 switch between FY17 and FY18
</commit_message>
<xml_diff>
--- a/computing_model_2016-11.xlsx
+++ b/computing_model_2016-11.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="154">
   <si>
     <t>GlueX Computing Model</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>MC CPU time per event, generation</t>
+  </si>
+  <si>
+    <t>per David's email of 11/1, point 2, fy 18 a factor of two more due to G3 → G4 switch</t>
   </si>
   <si>
     <t>MC CPU time per event, reconstruction</t>
@@ -695,7 +698,7 @@
   <dimension ref="1:65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1153,13 +1156,16 @@
         <v>0.0555555555555556</v>
       </c>
       <c r="C28" s="3" t="n">
-        <f aca="false">1/18</f>
-        <v>0.0555555555555556</v>
+        <f aca="false">2*(1/18)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">B9</f>
@@ -1172,7 +1178,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">B28/B9</f>
@@ -1180,18 +1186,18 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C28/C9</f>
-        <v>0.544444444444444</v>
+        <v>1.08888888888888</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">B29/B9</f>
@@ -1202,12 +1208,12 @@
         <v>1</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3" t="n">
         <v>2</v>
@@ -1216,12 +1222,12 @@
         <v>2</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>18000</v>
@@ -1233,12 +1239,12 @@
         <v>25</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3" t="n">
         <v>2</v>
@@ -1247,12 +1253,12 @@
         <v>2</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B7*B32*B34</f>
@@ -1266,12 +1272,12 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">B32*B10*(B30+B31)*B34</f>
@@ -1279,18 +1285,18 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C32*C10*(C30+C31)*C34</f>
-        <v>3149.77006088768</v>
+        <v>4260.12065789125</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B37" s="0" t="n">
         <f aca="false">B33*B48</f>
@@ -1304,12 +1310,12 @@
         <v>25</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B38" s="0" t="n">
         <f aca="false">B35*B37/1000000</f>
@@ -1325,7 +1331,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B39" s="0" t="n">
         <f aca="false">B38*$F2/1000000000</f>
@@ -1341,7 +1347,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" s="3" t="n">
         <v>0.1</v>
@@ -1350,12 +1356,12 @@
         <v>0.1</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B41" s="3" t="n">
         <v>10</v>
@@ -1364,12 +1370,12 @@
         <v>10</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B42" s="0" t="n">
         <f aca="false">B40*B10*B41</f>
@@ -1383,12 +1389,12 @@
         <v>22</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B43" s="9" t="n">
         <f aca="false">B18+B19+B25+B36+B42</f>
@@ -1396,19 +1402,19 @@
       </c>
       <c r="C43" s="9" t="n">
         <f aca="false">C18+C19+C25+C36+C42</f>
-        <v>5240.1750113689</v>
+        <v>6350.52560837247</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AMJ43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44" s="0" t="n">
         <f aca="false">B43-B36</f>
@@ -1416,18 +1422,18 @@
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">C43-C36</f>
-        <v>2090.40495048121</v>
+        <v>2090.40495048122</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B45" s="3" t="n">
         <v>100</v>
@@ -1439,12 +1445,12 @@
         <v>28</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="n">
         <v>3</v>
@@ -1456,12 +1462,12 @@
         <v>28</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B47" s="0" t="n">
         <f aca="false">B7*B11/B45/1000000</f>
@@ -1474,7 +1480,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B48" s="3" t="n">
         <v>0.2</v>
@@ -1483,12 +1489,12 @@
         <v>0.2</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B49" s="0" t="n">
         <f aca="false">B48*B11</f>
@@ -1502,12 +1508,12 @@
         <v>25</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B50" s="0" t="n">
         <f aca="false">B7*B49/1000000</f>
@@ -1521,12 +1527,12 @@
         <v>28</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B51" s="0" t="n">
         <f aca="false">B16*B50*365.25*24*60*60/1000000000</f>
@@ -1540,12 +1546,12 @@
         <v>58</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B52" s="0" t="n">
         <f aca="false">B15*B7*B49/1000000</f>
@@ -1559,12 +1565,12 @@
         <v>28</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B53" s="0" t="n">
         <f aca="false">B17*B52*365.25*24*60*60/1000000000</f>
@@ -1578,12 +1584,12 @@
         <v>58</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B54" s="0" t="n">
         <f aca="false">B7*(B49+B11)/(B45*1000000)</f>
@@ -1594,15 +1600,15 @@
         <v>1.37905544147844</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B55" s="0" t="n">
         <f aca="false">B16*B54</f>
@@ -1613,15 +1619,15 @@
         <v>2.75811088295687</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B56" s="0" t="n">
         <f aca="false">B15*B54</f>
@@ -1632,15 +1638,15 @@
         <v>0.0689527720739218</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B57" s="0" t="n">
         <f aca="false">B17*B56</f>
@@ -1651,15 +1657,15 @@
         <v>0.137905544147844</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B58" s="0" t="n">
         <f aca="false">B7*B49/(10*1000000)</f>
@@ -1670,15 +1676,15 @@
         <v>2.29842573579739</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B59" s="0" t="n">
         <f aca="false">B22*B58*B20</f>
@@ -1689,15 +1695,15 @@
         <v>1.1492128678987</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B60" s="0" t="n">
         <f aca="false">(B58+B59)*B24</f>
@@ -1708,15 +1714,15 @@
         <v>6.89527720739218</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B61" s="0" t="n">
         <f aca="false">B38/B45</f>
@@ -1727,15 +1733,15 @@
         <v>0.719507186858314</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B62" s="0" t="n">
         <f aca="false">B47+B55+B57+B60+B61</f>
@@ -1746,12 +1752,12 @@
         <v>11.6600136892539</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B63" s="3" t="n">
         <v>20</v>
@@ -1760,15 +1766,15 @@
         <v>20</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B64" s="0" t="n">
         <f aca="false">B63*B41</f>
@@ -1779,15 +1785,15 @@
         <v>200</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B65" s="0" t="n">
         <f aca="false">B14/1000+B51+B53+B27+B39</f>
@@ -1839,7 +1845,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B2" s="3" t="n">
         <f aca="false">model!B5</f>
@@ -1852,7 +1858,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">7*B2</f>
@@ -1863,7 +1869,7 @@
         <v>73</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>2</v>
@@ -1871,7 +1877,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">model!B6</f>
@@ -1882,7 +1888,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">24*60*60</f>
@@ -1891,7 +1897,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B5" s="5" t="n">
         <f aca="false">B3*B4*$E$4</f>
@@ -1902,7 +1908,7 @@
         <v>3153600</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>365.25</v>
@@ -1910,7 +1916,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>20000</v>
@@ -1919,7 +1925,7 @@
         <v>20000</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>10000</v>
@@ -1927,7 +1933,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B7" s="5" t="n">
         <f aca="false">B5*B6</f>
@@ -1938,7 +1944,7 @@
         <v>63072000000</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2</v>
@@ -1948,7 +1954,7 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>18000</v>
@@ -1956,7 +1962,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">model!B9</f>
@@ -1967,7 +1973,7 @@
         <v>0.102040816326531</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.2</v>
@@ -1975,7 +1981,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B7*B9/$E$4/$E$5</f>
@@ -1988,7 +1994,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B7*B9/$E$4/$E$6</f>
@@ -2001,7 +2007,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">model!B28</f>
@@ -2009,12 +2015,12 @@
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">model!C28</f>
-        <v>0.0555555555555556</v>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">B9</f>
@@ -2027,7 +2033,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">B7*$E$7*(B14+B13)/$E$4/$E$6</f>
@@ -2035,12 +2041,12 @@
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">C7*$E$7*(C14+C13)/$E$4/$E$6</f>
-        <v>23.0090702947846</v>
+        <v>31.1201814058957</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">B11+B15</f>
@@ -2048,12 +2054,12 @@
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">C11+C15</f>
-        <v>30.4580498866213</v>
+        <v>38.5691609977325</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B7*$E8</f>
@@ -2066,7 +2072,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B23/1E+015</f>
@@ -2079,7 +2085,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B25" s="0" t="n">
         <f aca="false">B24*$E9</f>
@@ -2092,7 +2098,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">B24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>

</xml_diff>

<commit_message>
row 9 of the spreadsheet from: Oct 2016 David benchmark to Oct 2016 David benchmark 2016-Broadwell real cores
</commit_message>
<xml_diff>
--- a/computing_model_2016-11.xlsx
+++ b/computing_model_2016-11.xlsx
@@ -81,7 +81,7 @@
     <t>CPU-s/event</t>
   </si>
   <si>
-    <t>Oct. 2016 David benchmark</t>
+    <t>Oct. 2016 David benchmark 2016-Broadwell real cores</t>
   </si>
   <si>
     <t>single Pass 1 CPU needed</t>
@@ -698,7 +698,7 @@
   <dimension ref="1:65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>